<commit_message>
Excel, dataProvider and login tests
</commit_message>
<xml_diff>
--- a/src/test/resources/TestData/dsAlgo_TestData.xlsx
+++ b/src/test/resources/TestData/dsAlgo_TestData.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28623"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28730"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\skurr\eclipse-workspace\ClubNinjas-dsAlgoBDD\src\test\resources\TestData\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\skurr\eclipse-workspace\ClubNinjas-dsAlgoTestNG\src\test\resources\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EE4A0B10-8925-4351-B15D-69B74E3DB248}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CBAF166E-30D5-4216-B215-422253CC6E72}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3650" yWindow="1960" windowWidth="14400" windowHeight="7310" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Register" sheetId="2" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="146" uniqueCount="76">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="153" uniqueCount="80">
   <si>
     <t>UserName</t>
   </si>
@@ -293,6 +293,18 @@
   </si>
   <si>
     <t>Empty</t>
+  </si>
+  <si>
+    <t>scenario</t>
+  </si>
+  <si>
+    <t>validLoginId</t>
+  </si>
+  <si>
+    <t>invalidLogin</t>
+  </si>
+  <si>
+    <t>EmptyField</t>
   </si>
 </sst>
 </file>
@@ -2058,37 +2070,44 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D19390E6-AB14-4B31-A0B5-2F88190D0871}">
-  <dimension ref="A1:B2"/>
+  <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="16.1796875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15.6328125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.7265625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.1796875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.6328125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A1" s="13" t="s">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A1" t="s">
+        <v>76</v>
+      </c>
+      <c r="B1" s="13" t="s">
         <v>27</v>
       </c>
-      <c r="B1" s="13" t="s">
+      <c r="C1" s="13" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A2" s="14" t="s">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>77</v>
+      </c>
+      <c r="B2" s="14" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="C2" s="1" t="s">
         <v>2</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B2" r:id="rId1" xr:uid="{23CB3FB1-0FA9-48D0-85C1-1583AC770DBF}"/>
+    <hyperlink ref="C2" r:id="rId1" xr:uid="{23CB3FB1-0FA9-48D0-85C1-1583AC770DBF}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -2096,76 +2115,93 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D9"/>
+  <dimension ref="A1:E9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="22" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15.6328125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="20" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="51.08984375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.6328125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="22" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.6328125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="20" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="51.08984375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
+        <v>76</v>
+      </c>
+      <c r="B1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="B2" t="s">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>79</v>
+      </c>
+      <c r="C2" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="1"/>
-      <c r="D2" s="2"/>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="D2" s="1"/>
+      <c r="E2" s="2"/>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
+        <v>79</v>
+      </c>
+      <c r="B3" t="s">
         <v>3</v>
       </c>
-      <c r="D3" s="2"/>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="E3" s="2"/>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
+        <v>78</v>
+      </c>
+      <c r="B4" t="s">
         <v>3</v>
       </c>
-      <c r="B4" t="s">
+      <c r="C4" t="s">
         <v>34</v>
       </c>
-      <c r="D4" s="2"/>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="E4" s="2"/>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
+        <v>78</v>
+      </c>
+      <c r="B5" t="s">
         <v>35</v>
       </c>
-      <c r="B5" s="1" t="s">
+      <c r="C5" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D5" s="2"/>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="D6" s="2"/>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="D7" s="2"/>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="D8" s="2"/>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="D9" s="2"/>
+      <c r="E5" s="2"/>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="E6" s="2"/>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="E7" s="2"/>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="E8" s="2"/>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="E9" s="2"/>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B5" r:id="rId1" xr:uid="{08128789-F0FF-4810-AFFE-2FF1C73369F4}"/>
+    <hyperlink ref="C5" r:id="rId1" xr:uid="{08128789-F0FF-4810-AFFE-2FF1C73369F4}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -2173,7 +2209,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B36287EC-5C35-4A53-A766-4648041612D3}">
   <dimension ref="A1:C7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Added ExtentReport and CrossBrowser
</commit_message>
<xml_diff>
--- a/src/test/resources/TestData/dsAlgo_TestData.xlsx
+++ b/src/test/resources/TestData/dsAlgo_TestData.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jimre\eclipse-workspace\DSAlgoTestNG_ClubNinjas\ClubNinjas_DsAlgoTestNG\src\test\resources\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9186A241-AA02-4767-A941-794D1FF1A526}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BEE685CD-807E-4096-9FD3-2DC1E055BB00}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="28996" windowHeight="15675" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="28996" windowHeight="15675" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Register" sheetId="2" r:id="rId1"/>
@@ -2108,7 +2108,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D19390E6-AB14-4B31-A0B5-2F88190D0871}">
   <dimension ref="A1:C2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="S16" sqref="S16"/>
     </sheetView>
   </sheetViews>
@@ -2407,8 +2407,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9C156544-10E3-4CC6-B021-D85ABA7773B9}">
   <dimension ref="A1:D13"/>
   <sheetViews>
-    <sheetView topLeftCell="A11" workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>

</xml_diff>